<commit_message>
rerun and extract cpsat and gurobi
</commit_message>
<xml_diff>
--- a/other-approaches/Gurobi/nrp_gurobi_exp_results.xlsx
+++ b/other-approaches/Gurobi/nrp_gurobi_exp_results.xlsx
@@ -472,10 +472,10 @@
         <v>1</v>
       </c>
       <c r="E2" t="n">
-        <v>0.02</v>
+        <v>0.017</v>
       </c>
       <c r="F2" t="n">
-        <v>10.51</v>
+        <v>10.48</v>
       </c>
     </row>
     <row r="3">
@@ -494,10 +494,10 @@
         <v>2</v>
       </c>
       <c r="E3" t="n">
-        <v>0.02</v>
+        <v>0.016</v>
       </c>
       <c r="F3" t="n">
-        <v>10.53</v>
+        <v>10.54</v>
       </c>
     </row>
     <row r="4">
@@ -516,10 +516,10 @@
         <v>3</v>
       </c>
       <c r="E4" t="n">
-        <v>0.02</v>
+        <v>0.016</v>
       </c>
       <c r="F4" t="n">
-        <v>10.47</v>
+        <v>10.54</v>
       </c>
     </row>
     <row r="5">
@@ -538,10 +538,10 @@
         <v>4</v>
       </c>
       <c r="E5" t="n">
-        <v>0.02</v>
+        <v>0.016</v>
       </c>
       <c r="F5" t="n">
-        <v>10.53</v>
+        <v>10.51</v>
       </c>
     </row>
     <row r="6">
@@ -560,10 +560,10 @@
         <v>5</v>
       </c>
       <c r="E6" t="n">
-        <v>0.02</v>
+        <v>0.017</v>
       </c>
       <c r="F6" t="n">
-        <v>10.62</v>
+        <v>10.54</v>
       </c>
     </row>
     <row r="7">
@@ -582,10 +582,10 @@
         <v>6</v>
       </c>
       <c r="E7" t="n">
-        <v>0.02</v>
+        <v>0.016</v>
       </c>
       <c r="F7" t="n">
-        <v>10.48</v>
+        <v>10.46</v>
       </c>
     </row>
     <row r="8">
@@ -604,7 +604,7 @@
         <v>7</v>
       </c>
       <c r="E8" t="n">
-        <v>0.02</v>
+        <v>0.017</v>
       </c>
       <c r="F8" t="n">
         <v>10.48</v>
@@ -626,10 +626,10 @@
         <v>8</v>
       </c>
       <c r="E9" t="n">
-        <v>0.02</v>
+        <v>0.017</v>
       </c>
       <c r="F9" t="n">
-        <v>10.47</v>
+        <v>10.48</v>
       </c>
     </row>
     <row r="10">
@@ -648,10 +648,10 @@
         <v>9</v>
       </c>
       <c r="E10" t="n">
-        <v>0.02</v>
+        <v>0.017</v>
       </c>
       <c r="F10" t="n">
-        <v>10.53</v>
+        <v>10.54</v>
       </c>
     </row>
     <row r="11">
@@ -670,10 +670,10 @@
         <v>10</v>
       </c>
       <c r="E11" t="n">
-        <v>0.02</v>
+        <v>0.016</v>
       </c>
       <c r="F11" t="n">
-        <v>10.53</v>
+        <v>10.48</v>
       </c>
     </row>
     <row r="12">
@@ -690,10 +690,10 @@
       </c>
       <c r="D12" t="inlineStr"/>
       <c r="E12" t="n">
-        <v>0.02</v>
+        <v>0.0165</v>
       </c>
       <c r="F12" t="n">
-        <v>10.515</v>
+        <v>10.505</v>
       </c>
     </row>
   </sheetData>
@@ -763,10 +763,10 @@
         <v>1</v>
       </c>
       <c r="E2" t="n">
-        <v>0.02</v>
+        <v>0.025</v>
       </c>
       <c r="F2" t="n">
-        <v>10.05</v>
+        <v>9.99</v>
       </c>
     </row>
     <row r="3">
@@ -785,10 +785,10 @@
         <v>2</v>
       </c>
       <c r="E3" t="n">
-        <v>0.03</v>
+        <v>0.025</v>
       </c>
       <c r="F3" t="n">
-        <v>10.05</v>
+        <v>9.890000000000001</v>
       </c>
     </row>
     <row r="4">
@@ -807,10 +807,10 @@
         <v>3</v>
       </c>
       <c r="E4" t="n">
-        <v>0.03</v>
+        <v>0.025</v>
       </c>
       <c r="F4" t="n">
-        <v>9.949999999999999</v>
+        <v>10.04</v>
       </c>
     </row>
     <row r="5">
@@ -829,10 +829,10 @@
         <v>4</v>
       </c>
       <c r="E5" t="n">
-        <v>0.02</v>
+        <v>0.025</v>
       </c>
       <c r="F5" t="n">
-        <v>10.01</v>
+        <v>10.02</v>
       </c>
     </row>
     <row r="6">
@@ -851,10 +851,10 @@
         <v>5</v>
       </c>
       <c r="E6" t="n">
-        <v>0.03</v>
+        <v>0.025</v>
       </c>
       <c r="F6" t="n">
-        <v>10.01</v>
+        <v>9.890000000000001</v>
       </c>
     </row>
     <row r="7">
@@ -873,10 +873,10 @@
         <v>6</v>
       </c>
       <c r="E7" t="n">
-        <v>0.03</v>
+        <v>0.025</v>
       </c>
       <c r="F7" t="n">
-        <v>10</v>
+        <v>9.94</v>
       </c>
     </row>
     <row r="8">
@@ -895,10 +895,10 @@
         <v>7</v>
       </c>
       <c r="E8" t="n">
-        <v>0.03</v>
+        <v>0.025</v>
       </c>
       <c r="F8" t="n">
-        <v>10.01</v>
+        <v>10</v>
       </c>
     </row>
     <row r="9">
@@ -917,10 +917,10 @@
         <v>8</v>
       </c>
       <c r="E9" t="n">
-        <v>0.02</v>
+        <v>0.025</v>
       </c>
       <c r="F9" t="n">
-        <v>10.03</v>
+        <v>9.99</v>
       </c>
     </row>
     <row r="10">
@@ -939,10 +939,10 @@
         <v>9</v>
       </c>
       <c r="E10" t="n">
-        <v>0.02</v>
+        <v>0.027</v>
       </c>
       <c r="F10" t="n">
-        <v>9.890000000000001</v>
+        <v>10.02</v>
       </c>
     </row>
     <row r="11">
@@ -961,10 +961,10 @@
         <v>10</v>
       </c>
       <c r="E11" t="n">
-        <v>0.02</v>
+        <v>0.025</v>
       </c>
       <c r="F11" t="n">
-        <v>10.01</v>
+        <v>10.03</v>
       </c>
     </row>
     <row r="12">
@@ -981,10 +981,10 @@
       </c>
       <c r="D12" t="inlineStr"/>
       <c r="E12" t="n">
-        <v>0.025</v>
+        <v>0.0252</v>
       </c>
       <c r="F12" t="n">
-        <v>10.001</v>
+        <v>9.980999999999998</v>
       </c>
     </row>
   </sheetData>
@@ -1054,10 +1054,10 @@
         <v>1</v>
       </c>
       <c r="E2" t="n">
-        <v>0.04</v>
+        <v>0.038</v>
       </c>
       <c r="F2" t="n">
-        <v>13.57</v>
+        <v>13.51</v>
       </c>
     </row>
     <row r="3">
@@ -1076,10 +1076,10 @@
         <v>2</v>
       </c>
       <c r="E3" t="n">
-        <v>0.04</v>
+        <v>0.038</v>
       </c>
       <c r="F3" t="n">
-        <v>13.57</v>
+        <v>13.55</v>
       </c>
     </row>
     <row r="4">
@@ -1098,10 +1098,10 @@
         <v>3</v>
       </c>
       <c r="E4" t="n">
-        <v>0.04</v>
+        <v>0.039</v>
       </c>
       <c r="F4" t="n">
-        <v>13.58</v>
+        <v>13.51</v>
       </c>
     </row>
     <row r="5">
@@ -1120,10 +1120,10 @@
         <v>4</v>
       </c>
       <c r="E5" t="n">
-        <v>0.04</v>
+        <v>0.038</v>
       </c>
       <c r="F5" t="n">
-        <v>13.61</v>
+        <v>13.5</v>
       </c>
     </row>
     <row r="6">
@@ -1142,10 +1142,10 @@
         <v>5</v>
       </c>
       <c r="E6" t="n">
-        <v>0.04</v>
+        <v>0.039</v>
       </c>
       <c r="F6" t="n">
-        <v>13.5</v>
+        <v>13.57</v>
       </c>
     </row>
     <row r="7">
@@ -1164,10 +1164,10 @@
         <v>6</v>
       </c>
       <c r="E7" t="n">
-        <v>0.04</v>
+        <v>0.038</v>
       </c>
       <c r="F7" t="n">
-        <v>13.55</v>
+        <v>13.59</v>
       </c>
     </row>
     <row r="8">
@@ -1189,7 +1189,7 @@
         <v>0.04</v>
       </c>
       <c r="F8" t="n">
-        <v>13.52</v>
+        <v>13.56</v>
       </c>
     </row>
     <row r="9">
@@ -1208,10 +1208,10 @@
         <v>8</v>
       </c>
       <c r="E9" t="n">
-        <v>0.04</v>
+        <v>0.039</v>
       </c>
       <c r="F9" t="n">
-        <v>13.51</v>
+        <v>13.65</v>
       </c>
     </row>
     <row r="10">
@@ -1230,10 +1230,10 @@
         <v>9</v>
       </c>
       <c r="E10" t="n">
-        <v>0.04</v>
+        <v>0.039</v>
       </c>
       <c r="F10" t="n">
-        <v>13.45</v>
+        <v>13.57</v>
       </c>
     </row>
     <row r="11">
@@ -1252,10 +1252,10 @@
         <v>10</v>
       </c>
       <c r="E11" t="n">
-        <v>0.04</v>
+        <v>0.039</v>
       </c>
       <c r="F11" t="n">
-        <v>13.65</v>
+        <v>13.56</v>
       </c>
     </row>
     <row r="12">
@@ -1272,10 +1272,10 @@
       </c>
       <c r="D12" t="inlineStr"/>
       <c r="E12" t="n">
-        <v>0.03999999999999999</v>
+        <v>0.0387</v>
       </c>
       <c r="F12" t="n">
-        <v>13.551</v>
+        <v>13.557</v>
       </c>
     </row>
   </sheetData>
@@ -1345,10 +1345,10 @@
         <v>1</v>
       </c>
       <c r="E2" t="n">
-        <v>0.06</v>
+        <v>0.057</v>
       </c>
       <c r="F2" t="n">
-        <v>11.6</v>
+        <v>11.61</v>
       </c>
     </row>
     <row r="3">
@@ -1367,10 +1367,10 @@
         <v>2</v>
       </c>
       <c r="E3" t="n">
-        <v>0.06</v>
+        <v>0.056</v>
       </c>
       <c r="F3" t="n">
-        <v>11.64</v>
+        <v>11.61</v>
       </c>
     </row>
     <row r="4">
@@ -1389,7 +1389,7 @@
         <v>3</v>
       </c>
       <c r="E4" t="n">
-        <v>0.06</v>
+        <v>0.056</v>
       </c>
       <c r="F4" t="n">
         <v>11.61</v>
@@ -1411,10 +1411,10 @@
         <v>4</v>
       </c>
       <c r="E5" t="n">
-        <v>0.06</v>
+        <v>0.056</v>
       </c>
       <c r="F5" t="n">
-        <v>11.61</v>
+        <v>11.69</v>
       </c>
     </row>
     <row r="6">
@@ -1433,10 +1433,10 @@
         <v>5</v>
       </c>
       <c r="E6" t="n">
-        <v>0.06</v>
+        <v>0.056</v>
       </c>
       <c r="F6" t="n">
-        <v>11.6</v>
+        <v>11.61</v>
       </c>
     </row>
     <row r="7">
@@ -1455,10 +1455,10 @@
         <v>6</v>
       </c>
       <c r="E7" t="n">
-        <v>0.06</v>
+        <v>0.056</v>
       </c>
       <c r="F7" t="n">
-        <v>11.62</v>
+        <v>11.55</v>
       </c>
     </row>
     <row r="8">
@@ -1477,10 +1477,10 @@
         <v>7</v>
       </c>
       <c r="E8" t="n">
-        <v>0.06</v>
+        <v>0.057</v>
       </c>
       <c r="F8" t="n">
-        <v>11.55</v>
+        <v>11.63</v>
       </c>
     </row>
     <row r="9">
@@ -1499,10 +1499,10 @@
         <v>8</v>
       </c>
       <c r="E9" t="n">
-        <v>0.06</v>
+        <v>0.056</v>
       </c>
       <c r="F9" t="n">
-        <v>11.61</v>
+        <v>11.6</v>
       </c>
     </row>
     <row r="10">
@@ -1521,10 +1521,10 @@
         <v>9</v>
       </c>
       <c r="E10" t="n">
-        <v>0.06</v>
+        <v>0.057</v>
       </c>
       <c r="F10" t="n">
-        <v>11.6</v>
+        <v>11.55</v>
       </c>
     </row>
     <row r="11">
@@ -1543,10 +1543,10 @@
         <v>10</v>
       </c>
       <c r="E11" t="n">
-        <v>0.06</v>
+        <v>0.057</v>
       </c>
       <c r="F11" t="n">
-        <v>11.6</v>
+        <v>11.62</v>
       </c>
     </row>
     <row r="12">
@@ -1563,10 +1563,10 @@
       </c>
       <c r="D12" t="inlineStr"/>
       <c r="E12" t="n">
-        <v>0.06000000000000001</v>
+        <v>0.05640000000000001</v>
       </c>
       <c r="F12" t="n">
-        <v>11.604</v>
+        <v>11.608</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
rerun gurobi with academic license
</commit_message>
<xml_diff>
--- a/other-approaches/Gurobi/nrp_gurobi_exp_results.xlsx
+++ b/other-approaches/Gurobi/nrp_gurobi_exp_results.xlsx
@@ -472,10 +472,10 @@
         <v>1</v>
       </c>
       <c r="E2" t="n">
-        <v>0.017</v>
+        <v>0.422</v>
       </c>
       <c r="F2" t="n">
-        <v>10.48</v>
+        <v>16.5</v>
       </c>
     </row>
     <row r="3">
@@ -494,10 +494,10 @@
         <v>2</v>
       </c>
       <c r="E3" t="n">
-        <v>0.016</v>
+        <v>0.017</v>
       </c>
       <c r="F3" t="n">
-        <v>10.54</v>
+        <v>15.39</v>
       </c>
     </row>
     <row r="4">
@@ -516,10 +516,10 @@
         <v>3</v>
       </c>
       <c r="E4" t="n">
-        <v>0.016</v>
+        <v>0.017</v>
       </c>
       <c r="F4" t="n">
-        <v>10.54</v>
+        <v>15.27</v>
       </c>
     </row>
     <row r="5">
@@ -538,10 +538,10 @@
         <v>4</v>
       </c>
       <c r="E5" t="n">
-        <v>0.016</v>
+        <v>0.017</v>
       </c>
       <c r="F5" t="n">
-        <v>10.51</v>
+        <v>15.41</v>
       </c>
     </row>
     <row r="6">
@@ -563,7 +563,7 @@
         <v>0.017</v>
       </c>
       <c r="F6" t="n">
-        <v>10.54</v>
+        <v>15.46</v>
       </c>
     </row>
     <row r="7">
@@ -582,10 +582,10 @@
         <v>6</v>
       </c>
       <c r="E7" t="n">
-        <v>0.016</v>
+        <v>0.018</v>
       </c>
       <c r="F7" t="n">
-        <v>10.46</v>
+        <v>15.41</v>
       </c>
     </row>
     <row r="8">
@@ -604,10 +604,10 @@
         <v>7</v>
       </c>
       <c r="E8" t="n">
-        <v>0.017</v>
+        <v>0.018</v>
       </c>
       <c r="F8" t="n">
-        <v>10.48</v>
+        <v>15.34</v>
       </c>
     </row>
     <row r="9">
@@ -626,10 +626,10 @@
         <v>8</v>
       </c>
       <c r="E9" t="n">
-        <v>0.017</v>
+        <v>0.018</v>
       </c>
       <c r="F9" t="n">
-        <v>10.48</v>
+        <v>15.46</v>
       </c>
     </row>
     <row r="10">
@@ -648,10 +648,10 @@
         <v>9</v>
       </c>
       <c r="E10" t="n">
-        <v>0.017</v>
+        <v>0.019</v>
       </c>
       <c r="F10" t="n">
-        <v>10.54</v>
+        <v>15.46</v>
       </c>
     </row>
     <row r="11">
@@ -670,10 +670,10 @@
         <v>10</v>
       </c>
       <c r="E11" t="n">
-        <v>0.016</v>
+        <v>0.017</v>
       </c>
       <c r="F11" t="n">
-        <v>10.48</v>
+        <v>15.48</v>
       </c>
     </row>
     <row r="12">
@@ -690,10 +690,10 @@
       </c>
       <c r="D12" t="inlineStr"/>
       <c r="E12" t="n">
-        <v>0.0165</v>
+        <v>0.05800000000000001</v>
       </c>
       <c r="F12" t="n">
-        <v>10.505</v>
+        <v>15.518</v>
       </c>
     </row>
   </sheetData>
@@ -763,10 +763,10 @@
         <v>1</v>
       </c>
       <c r="E2" t="n">
-        <v>0.025</v>
+        <v>0.026</v>
       </c>
       <c r="F2" t="n">
-        <v>9.99</v>
+        <v>14.91</v>
       </c>
     </row>
     <row r="3">
@@ -785,10 +785,10 @@
         <v>2</v>
       </c>
       <c r="E3" t="n">
-        <v>0.025</v>
+        <v>0.026</v>
       </c>
       <c r="F3" t="n">
-        <v>9.890000000000001</v>
+        <v>14.92</v>
       </c>
     </row>
     <row r="4">
@@ -807,10 +807,10 @@
         <v>3</v>
       </c>
       <c r="E4" t="n">
-        <v>0.025</v>
+        <v>0.027</v>
       </c>
       <c r="F4" t="n">
-        <v>10.04</v>
+        <v>14.92</v>
       </c>
     </row>
     <row r="5">
@@ -829,10 +829,10 @@
         <v>4</v>
       </c>
       <c r="E5" t="n">
-        <v>0.025</v>
+        <v>0.026</v>
       </c>
       <c r="F5" t="n">
-        <v>10.02</v>
+        <v>14.87</v>
       </c>
     </row>
     <row r="6">
@@ -851,10 +851,10 @@
         <v>5</v>
       </c>
       <c r="E6" t="n">
-        <v>0.025</v>
+        <v>0.026</v>
       </c>
       <c r="F6" t="n">
-        <v>9.890000000000001</v>
+        <v>14.94</v>
       </c>
     </row>
     <row r="7">
@@ -873,10 +873,10 @@
         <v>6</v>
       </c>
       <c r="E7" t="n">
-        <v>0.025</v>
+        <v>0.026</v>
       </c>
       <c r="F7" t="n">
-        <v>9.94</v>
+        <v>14.73</v>
       </c>
     </row>
     <row r="8">
@@ -895,10 +895,10 @@
         <v>7</v>
       </c>
       <c r="E8" t="n">
-        <v>0.025</v>
+        <v>0.027</v>
       </c>
       <c r="F8" t="n">
-        <v>10</v>
+        <v>14.86</v>
       </c>
     </row>
     <row r="9">
@@ -917,10 +917,10 @@
         <v>8</v>
       </c>
       <c r="E9" t="n">
-        <v>0.025</v>
+        <v>0.026</v>
       </c>
       <c r="F9" t="n">
-        <v>9.99</v>
+        <v>14.8</v>
       </c>
     </row>
     <row r="10">
@@ -939,10 +939,10 @@
         <v>9</v>
       </c>
       <c r="E10" t="n">
-        <v>0.027</v>
+        <v>0.026</v>
       </c>
       <c r="F10" t="n">
-        <v>10.02</v>
+        <v>14.79</v>
       </c>
     </row>
     <row r="11">
@@ -961,10 +961,10 @@
         <v>10</v>
       </c>
       <c r="E11" t="n">
-        <v>0.025</v>
+        <v>0.026</v>
       </c>
       <c r="F11" t="n">
-        <v>10.03</v>
+        <v>14.84</v>
       </c>
     </row>
     <row r="12">
@@ -981,10 +981,10 @@
       </c>
       <c r="D12" t="inlineStr"/>
       <c r="E12" t="n">
-        <v>0.0252</v>
+        <v>0.0262</v>
       </c>
       <c r="F12" t="n">
-        <v>9.980999999999998</v>
+        <v>14.858</v>
       </c>
     </row>
   </sheetData>
@@ -1054,10 +1054,10 @@
         <v>1</v>
       </c>
       <c r="E2" t="n">
-        <v>0.038</v>
+        <v>0.04</v>
       </c>
       <c r="F2" t="n">
-        <v>13.51</v>
+        <v>18.41</v>
       </c>
     </row>
     <row r="3">
@@ -1076,10 +1076,10 @@
         <v>2</v>
       </c>
       <c r="E3" t="n">
-        <v>0.038</v>
+        <v>0.04</v>
       </c>
       <c r="F3" t="n">
-        <v>13.55</v>
+        <v>18.47</v>
       </c>
     </row>
     <row r="4">
@@ -1101,7 +1101,7 @@
         <v>0.039</v>
       </c>
       <c r="F4" t="n">
-        <v>13.51</v>
+        <v>18.34</v>
       </c>
     </row>
     <row r="5">
@@ -1120,10 +1120,10 @@
         <v>4</v>
       </c>
       <c r="E5" t="n">
-        <v>0.038</v>
+        <v>0.039</v>
       </c>
       <c r="F5" t="n">
-        <v>13.5</v>
+        <v>18.46</v>
       </c>
     </row>
     <row r="6">
@@ -1142,10 +1142,10 @@
         <v>5</v>
       </c>
       <c r="E6" t="n">
-        <v>0.039</v>
+        <v>0.04</v>
       </c>
       <c r="F6" t="n">
-        <v>13.57</v>
+        <v>18.34</v>
       </c>
     </row>
     <row r="7">
@@ -1164,10 +1164,10 @@
         <v>6</v>
       </c>
       <c r="E7" t="n">
-        <v>0.038</v>
+        <v>0.039</v>
       </c>
       <c r="F7" t="n">
-        <v>13.59</v>
+        <v>18.42</v>
       </c>
     </row>
     <row r="8">
@@ -1186,10 +1186,10 @@
         <v>7</v>
       </c>
       <c r="E8" t="n">
-        <v>0.04</v>
+        <v>0.039</v>
       </c>
       <c r="F8" t="n">
-        <v>13.56</v>
+        <v>18.39</v>
       </c>
     </row>
     <row r="9">
@@ -1211,7 +1211,7 @@
         <v>0.039</v>
       </c>
       <c r="F9" t="n">
-        <v>13.65</v>
+        <v>18.48</v>
       </c>
     </row>
     <row r="10">
@@ -1233,7 +1233,7 @@
         <v>0.039</v>
       </c>
       <c r="F10" t="n">
-        <v>13.57</v>
+        <v>18.41</v>
       </c>
     </row>
     <row r="11">
@@ -1252,10 +1252,10 @@
         <v>10</v>
       </c>
       <c r="E11" t="n">
-        <v>0.039</v>
+        <v>0.04</v>
       </c>
       <c r="F11" t="n">
-        <v>13.56</v>
+        <v>18.42</v>
       </c>
     </row>
     <row r="12">
@@ -1272,10 +1272,10 @@
       </c>
       <c r="D12" t="inlineStr"/>
       <c r="E12" t="n">
-        <v>0.0387</v>
+        <v>0.0394</v>
       </c>
       <c r="F12" t="n">
-        <v>13.557</v>
+        <v>18.414</v>
       </c>
     </row>
   </sheetData>
@@ -1345,10 +1345,10 @@
         <v>1</v>
       </c>
       <c r="E2" t="n">
-        <v>0.057</v>
+        <v>0.061</v>
       </c>
       <c r="F2" t="n">
-        <v>11.61</v>
+        <v>16.48</v>
       </c>
     </row>
     <row r="3">
@@ -1367,10 +1367,10 @@
         <v>2</v>
       </c>
       <c r="E3" t="n">
-        <v>0.056</v>
+        <v>0.058</v>
       </c>
       <c r="F3" t="n">
-        <v>11.61</v>
+        <v>16.44</v>
       </c>
     </row>
     <row r="4">
@@ -1389,10 +1389,10 @@
         <v>3</v>
       </c>
       <c r="E4" t="n">
-        <v>0.056</v>
+        <v>0.058</v>
       </c>
       <c r="F4" t="n">
-        <v>11.61</v>
+        <v>16.33</v>
       </c>
     </row>
     <row r="5">
@@ -1411,10 +1411,10 @@
         <v>4</v>
       </c>
       <c r="E5" t="n">
-        <v>0.056</v>
+        <v>0.058</v>
       </c>
       <c r="F5" t="n">
-        <v>11.69</v>
+        <v>16.33</v>
       </c>
     </row>
     <row r="6">
@@ -1433,10 +1433,10 @@
         <v>5</v>
       </c>
       <c r="E6" t="n">
-        <v>0.056</v>
+        <v>0.058</v>
       </c>
       <c r="F6" t="n">
-        <v>11.61</v>
+        <v>16.47</v>
       </c>
     </row>
     <row r="7">
@@ -1455,10 +1455,10 @@
         <v>6</v>
       </c>
       <c r="E7" t="n">
-        <v>0.056</v>
+        <v>0.058</v>
       </c>
       <c r="F7" t="n">
-        <v>11.55</v>
+        <v>16.53</v>
       </c>
     </row>
     <row r="8">
@@ -1477,10 +1477,10 @@
         <v>7</v>
       </c>
       <c r="E8" t="n">
-        <v>0.057</v>
+        <v>0.058</v>
       </c>
       <c r="F8" t="n">
-        <v>11.63</v>
+        <v>16.47</v>
       </c>
     </row>
     <row r="9">
@@ -1499,10 +1499,10 @@
         <v>8</v>
       </c>
       <c r="E9" t="n">
-        <v>0.056</v>
+        <v>0.057</v>
       </c>
       <c r="F9" t="n">
-        <v>11.6</v>
+        <v>16.44</v>
       </c>
     </row>
     <row r="10">
@@ -1521,10 +1521,10 @@
         <v>9</v>
       </c>
       <c r="E10" t="n">
-        <v>0.057</v>
+        <v>0.058</v>
       </c>
       <c r="F10" t="n">
-        <v>11.55</v>
+        <v>16.33</v>
       </c>
     </row>
     <row r="11">
@@ -1543,10 +1543,10 @@
         <v>10</v>
       </c>
       <c r="E11" t="n">
-        <v>0.057</v>
+        <v>0.058</v>
       </c>
       <c r="F11" t="n">
-        <v>11.62</v>
+        <v>16.46</v>
       </c>
     </row>
     <row r="12">
@@ -1563,10 +1563,10 @@
       </c>
       <c r="D12" t="inlineStr"/>
       <c r="E12" t="n">
-        <v>0.05640000000000001</v>
+        <v>0.05820000000000001</v>
       </c>
       <c r="F12" t="n">
-        <v>11.608</v>
+        <v>16.428</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
only measure encoding and solving time of gurobi & rerun gurobi
</commit_message>
<xml_diff>
--- a/other-approaches/Gurobi/nrp_gurobi_exp_results.xlsx
+++ b/other-approaches/Gurobi/nrp_gurobi_exp_results.xlsx
@@ -472,10 +472,10 @@
         <v>1</v>
       </c>
       <c r="E2" t="n">
-        <v>0.018</v>
+        <v>0.508</v>
       </c>
       <c r="F2" t="n">
-        <v>15.51</v>
+        <v>16.77</v>
       </c>
     </row>
     <row r="3">
@@ -497,7 +497,7 @@
         <v>0.018</v>
       </c>
       <c r="F3" t="n">
-        <v>15.37</v>
+        <v>15.39</v>
       </c>
     </row>
     <row r="4">
@@ -516,7 +516,7 @@
         <v>3</v>
       </c>
       <c r="E4" t="n">
-        <v>0.017</v>
+        <v>0.019</v>
       </c>
       <c r="F4" t="n">
         <v>15.32</v>
@@ -538,10 +538,10 @@
         <v>4</v>
       </c>
       <c r="E5" t="n">
-        <v>0.017</v>
+        <v>0.019</v>
       </c>
       <c r="F5" t="n">
-        <v>15.3</v>
+        <v>15.26</v>
       </c>
     </row>
     <row r="6">
@@ -560,10 +560,10 @@
         <v>5</v>
       </c>
       <c r="E6" t="n">
-        <v>0.018</v>
+        <v>0.019</v>
       </c>
       <c r="F6" t="n">
-        <v>15.3</v>
+        <v>15.39</v>
       </c>
     </row>
     <row r="7">
@@ -585,7 +585,7 @@
         <v>0.018</v>
       </c>
       <c r="F7" t="n">
-        <v>15.43</v>
+        <v>15.45</v>
       </c>
     </row>
     <row r="8">
@@ -604,10 +604,10 @@
         <v>7</v>
       </c>
       <c r="E8" t="n">
-        <v>0.018</v>
+        <v>0.019</v>
       </c>
       <c r="F8" t="n">
-        <v>15.46</v>
+        <v>15.36</v>
       </c>
     </row>
     <row r="9">
@@ -629,7 +629,7 @@
         <v>0.018</v>
       </c>
       <c r="F9" t="n">
-        <v>15.45</v>
+        <v>15.4</v>
       </c>
     </row>
     <row r="10">
@@ -651,7 +651,7 @@
         <v>0.018</v>
       </c>
       <c r="F10" t="n">
-        <v>15.37</v>
+        <v>15.36</v>
       </c>
     </row>
     <row r="11">
@@ -673,7 +673,7 @@
         <v>0.018</v>
       </c>
       <c r="F11" t="n">
-        <v>15.47</v>
+        <v>15.37</v>
       </c>
     </row>
     <row r="12">
@@ -690,10 +690,10 @@
       </c>
       <c r="D12" t="inlineStr"/>
       <c r="E12" t="n">
-        <v>0.0178</v>
+        <v>0.0674</v>
       </c>
       <c r="F12" t="n">
-        <v>15.398</v>
+        <v>15.507</v>
       </c>
     </row>
   </sheetData>
@@ -763,10 +763,10 @@
         <v>1</v>
       </c>
       <c r="E2" t="n">
-        <v>0.026</v>
+        <v>0.028</v>
       </c>
       <c r="F2" t="n">
-        <v>14.87</v>
+        <v>14.86</v>
       </c>
     </row>
     <row r="3">
@@ -788,7 +788,7 @@
         <v>0.027</v>
       </c>
       <c r="F3" t="n">
-        <v>14.76</v>
+        <v>14.92</v>
       </c>
     </row>
     <row r="4">
@@ -810,7 +810,7 @@
         <v>0.026</v>
       </c>
       <c r="F4" t="n">
-        <v>14.97</v>
+        <v>14.86</v>
       </c>
     </row>
     <row r="5">
@@ -829,10 +829,10 @@
         <v>4</v>
       </c>
       <c r="E5" t="n">
-        <v>0.027</v>
+        <v>0.028</v>
       </c>
       <c r="F5" t="n">
-        <v>14.87</v>
+        <v>14.83</v>
       </c>
     </row>
     <row r="6">
@@ -854,7 +854,7 @@
         <v>0.027</v>
       </c>
       <c r="F6" t="n">
-        <v>14.83</v>
+        <v>14.78</v>
       </c>
     </row>
     <row r="7">
@@ -876,7 +876,7 @@
         <v>0.026</v>
       </c>
       <c r="F7" t="n">
-        <v>14.76</v>
+        <v>14.79</v>
       </c>
     </row>
     <row r="8">
@@ -895,10 +895,10 @@
         <v>7</v>
       </c>
       <c r="E8" t="n">
-        <v>0.026</v>
+        <v>0.028</v>
       </c>
       <c r="F8" t="n">
-        <v>14.87</v>
+        <v>14.85</v>
       </c>
     </row>
     <row r="9">
@@ -917,10 +917,10 @@
         <v>8</v>
       </c>
       <c r="E9" t="n">
-        <v>0.026</v>
+        <v>0.027</v>
       </c>
       <c r="F9" t="n">
-        <v>14.75</v>
+        <v>14.9</v>
       </c>
     </row>
     <row r="10">
@@ -939,10 +939,10 @@
         <v>9</v>
       </c>
       <c r="E10" t="n">
-        <v>0.027</v>
+        <v>0.026</v>
       </c>
       <c r="F10" t="n">
-        <v>14.9</v>
+        <v>14.86</v>
       </c>
     </row>
     <row r="11">
@@ -964,7 +964,7 @@
         <v>0.026</v>
       </c>
       <c r="F11" t="n">
-        <v>14.76</v>
+        <v>14.9</v>
       </c>
     </row>
     <row r="12">
@@ -981,10 +981,10 @@
       </c>
       <c r="D12" t="inlineStr"/>
       <c r="E12" t="n">
-        <v>0.0264</v>
+        <v>0.0269</v>
       </c>
       <c r="F12" t="n">
-        <v>14.834</v>
+        <v>14.855</v>
       </c>
     </row>
   </sheetData>
@@ -1057,7 +1057,7 @@
         <v>0.04</v>
       </c>
       <c r="F2" t="n">
-        <v>18.38</v>
+        <v>18.35</v>
       </c>
     </row>
     <row r="3">
@@ -1076,10 +1076,10 @@
         <v>2</v>
       </c>
       <c r="E3" t="n">
-        <v>0.04</v>
+        <v>0.041</v>
       </c>
       <c r="F3" t="n">
-        <v>18.42</v>
+        <v>18.39</v>
       </c>
     </row>
     <row r="4">
@@ -1098,10 +1098,10 @@
         <v>3</v>
       </c>
       <c r="E4" t="n">
-        <v>0.04</v>
+        <v>0.043</v>
       </c>
       <c r="F4" t="n">
-        <v>18.43</v>
+        <v>18.42</v>
       </c>
     </row>
     <row r="5">
@@ -1123,7 +1123,7 @@
         <v>0.04</v>
       </c>
       <c r="F5" t="n">
-        <v>18.31</v>
+        <v>18.27</v>
       </c>
     </row>
     <row r="6">
@@ -1145,7 +1145,7 @@
         <v>0.04</v>
       </c>
       <c r="F6" t="n">
-        <v>18.32</v>
+        <v>18.39</v>
       </c>
     </row>
     <row r="7">
@@ -1167,7 +1167,7 @@
         <v>0.04</v>
       </c>
       <c r="F7" t="n">
-        <v>18.31</v>
+        <v>18.28</v>
       </c>
     </row>
     <row r="8">
@@ -1189,7 +1189,7 @@
         <v>0.04</v>
       </c>
       <c r="F8" t="n">
-        <v>18.31</v>
+        <v>18.29</v>
       </c>
     </row>
     <row r="9">
@@ -1208,10 +1208,10 @@
         <v>8</v>
       </c>
       <c r="E9" t="n">
-        <v>0.041</v>
+        <v>0.039</v>
       </c>
       <c r="F9" t="n">
-        <v>18.42</v>
+        <v>18.28</v>
       </c>
     </row>
     <row r="10">
@@ -1230,10 +1230,10 @@
         <v>9</v>
       </c>
       <c r="E10" t="n">
-        <v>0.041</v>
+        <v>0.04</v>
       </c>
       <c r="F10" t="n">
-        <v>18.31</v>
+        <v>18.27</v>
       </c>
     </row>
     <row r="11">
@@ -1252,10 +1252,10 @@
         <v>10</v>
       </c>
       <c r="E11" t="n">
-        <v>0.039</v>
+        <v>0.041</v>
       </c>
       <c r="F11" t="n">
-        <v>18.3</v>
+        <v>18.39</v>
       </c>
     </row>
     <row r="12">
@@ -1272,10 +1272,10 @@
       </c>
       <c r="D12" t="inlineStr"/>
       <c r="E12" t="n">
-        <v>0.0401</v>
+        <v>0.04039999999999999</v>
       </c>
       <c r="F12" t="n">
-        <v>18.351</v>
+        <v>18.33300000000001</v>
       </c>
     </row>
   </sheetData>
@@ -1367,10 +1367,10 @@
         <v>2</v>
       </c>
       <c r="E3" t="n">
-        <v>0.06</v>
+        <v>0.061</v>
       </c>
       <c r="F3" t="n">
-        <v>16.5</v>
+        <v>16.4</v>
       </c>
     </row>
     <row r="4">
@@ -1389,10 +1389,10 @@
         <v>3</v>
       </c>
       <c r="E4" t="n">
-        <v>0.06</v>
+        <v>0.058</v>
       </c>
       <c r="F4" t="n">
-        <v>16.57</v>
+        <v>16.51</v>
       </c>
     </row>
     <row r="5">
@@ -1411,10 +1411,10 @@
         <v>4</v>
       </c>
       <c r="E5" t="n">
-        <v>0.057</v>
+        <v>0.059</v>
       </c>
       <c r="F5" t="n">
-        <v>16.5</v>
+        <v>16.44</v>
       </c>
     </row>
     <row r="6">
@@ -1433,10 +1433,10 @@
         <v>5</v>
       </c>
       <c r="E6" t="n">
-        <v>0.058</v>
+        <v>0.059</v>
       </c>
       <c r="F6" t="n">
-        <v>16.43</v>
+        <v>16.32</v>
       </c>
     </row>
     <row r="7">
@@ -1455,10 +1455,10 @@
         <v>6</v>
       </c>
       <c r="E7" t="n">
-        <v>0.057</v>
+        <v>0.059</v>
       </c>
       <c r="F7" t="n">
-        <v>16.42</v>
+        <v>16.33</v>
       </c>
     </row>
     <row r="8">
@@ -1477,10 +1477,10 @@
         <v>7</v>
       </c>
       <c r="E8" t="n">
-        <v>0.058</v>
+        <v>0.059</v>
       </c>
       <c r="F8" t="n">
-        <v>16.57</v>
+        <v>16.32</v>
       </c>
     </row>
     <row r="9">
@@ -1502,7 +1502,7 @@
         <v>0.059</v>
       </c>
       <c r="F9" t="n">
-        <v>16.51</v>
+        <v>16.32</v>
       </c>
     </row>
     <row r="10">
@@ -1524,7 +1524,7 @@
         <v>0.059</v>
       </c>
       <c r="F10" t="n">
-        <v>16.57</v>
+        <v>16.44</v>
       </c>
     </row>
     <row r="11">
@@ -1543,10 +1543,10 @@
         <v>10</v>
       </c>
       <c r="E11" t="n">
-        <v>0.061</v>
+        <v>0.059</v>
       </c>
       <c r="F11" t="n">
-        <v>16.48</v>
+        <v>16.44</v>
       </c>
     </row>
     <row r="12">
@@ -1563,10 +1563,10 @@
       </c>
       <c r="D12" t="inlineStr"/>
       <c r="E12" t="n">
-        <v>0.0587</v>
+        <v>0.05899999999999998</v>
       </c>
       <c r="F12" t="n">
-        <v>16.502</v>
+        <v>16.399</v>
       </c>
     </row>
   </sheetData>

</xml_diff>